<commit_message>
Began to develop pyrolysis geometry
</commit_message>
<xml_diff>
--- a/tests/Stove_test_Geometry.xlsx
+++ b/tests/Stove_test_Geometry.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oregon_State\Spring 2019\Soft_dev_eng\Project\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oregon_State\Spring_2019\Soft_dev_eng\StoveOpt\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1293FA7D-C438-4CBD-9E47-18A6E14F5DDC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2D61DC-1259-4841-8562-38F45AC80BB2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4272" yWindow="0" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{D0F77571-F344-4911-9ED7-19CABFB8BC85}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{D0F77571-F344-4911-9ED7-19CABFB8BC85}"/>
   </bookViews>
   <sheets>
     <sheet name="Purpose" sheetId="1" r:id="rId1"/>
@@ -1571,16 +1571,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>693420</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1744980</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>792480</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2672,8 +2672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F96E3B86-B810-49F2-ADC9-6B1B0C4097E0}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>